<commit_message>
pushing 5-5 from laptop
</commit_message>
<xml_diff>
--- a/Chip U/200mV Analysis/Number of Events.xlsx
+++ b/Chip U/200mV Analysis/Number of Events.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joshua Chen\Desktop\Other\GURU\Clampfit2\Chip U\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joshua Chen\Desktop\Other\GURU\Clampfit2\Chip U\200mV Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F9C41CA-EE6D-4562-BAC6-569D360FB638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7668170-61B2-4792-8C1F-F259CF3F4A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6D9A1C86-D149-4386-9463-DA16987C9825}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" activeTab="1" xr2:uid="{6D9A1C86-D149-4386-9463-DA16987C9825}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Data" sheetId="1" r:id="rId1"/>
     <sheet name="Ordered" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Ordered!$B$4:$I$161</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Ordered!$B$5:$I$162</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2432" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2433" uniqueCount="8">
   <si>
     <t>Uncategorized</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Percentage Events</t>
   </si>
 </sst>
 </file>
@@ -3747,15 +3750,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D83EDAD7-ABE3-4CBE-B6E6-396DDE8E1A3C}">
-  <dimension ref="A1:L222"/>
+  <dimension ref="A1:N223"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
       <c r="B1">
         <v>1</v>
       </c>
@@ -3789,8 +3792,11 @@
       <c r="L1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="N1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -3828,8 +3834,12 @@
         <f>SUM(B2:K2)</f>
         <v>98</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="N2">
+        <f>L2/L4</f>
+        <v>6.8917018284106887E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -3867,40 +3877,48 @@
         <f>SUM(B3:K3)</f>
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" t="s">
-        <v>1</v>
-      </c>
-      <c r="I4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J4" t="s">
-        <v>1</v>
-      </c>
-      <c r="K4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+      <c r="N3">
+        <f>L3/L4</f>
+        <v>7.0323488045007029E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="B4">
+        <v>116</v>
+      </c>
+      <c r="C4">
+        <v>108</v>
+      </c>
+      <c r="D4">
+        <v>133</v>
+      </c>
+      <c r="E4">
+        <v>150</v>
+      </c>
+      <c r="F4">
+        <v>119</v>
+      </c>
+      <c r="G4">
+        <v>125</v>
+      </c>
+      <c r="H4">
+        <v>116</v>
+      </c>
+      <c r="I4">
+        <v>140</v>
+      </c>
+      <c r="J4">
+        <v>196</v>
+      </c>
+      <c r="K4">
+        <v>219</v>
+      </c>
+      <c r="L4">
+        <f>SUM(B4:K4)</f>
+        <v>1422</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -3932,9 +3950,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
@@ -3964,7 +3982,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
         <v>1</v>
       </c>
@@ -3981,7 +3999,7 @@
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" t="s">
         <v>1</v>
@@ -3996,7 +4014,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
         <v>1</v>
       </c>
@@ -4025,10 +4043,10 @@
         <v>1</v>
       </c>
       <c r="K8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
         <v>1</v>
       </c>
@@ -4060,7 +4078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
       <c r="B10" t="s">
         <v>1</v>
       </c>
@@ -4068,7 +4086,7 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" t="s">
         <v>1</v>
@@ -4083,7 +4101,7 @@
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" t="s">
         <v>1</v>
@@ -4092,7 +4110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
       <c r="B11" t="s">
         <v>1</v>
       </c>
@@ -4103,10 +4121,10 @@
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" t="s">
         <v>0</v>
@@ -4118,13 +4136,13 @@
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
       <c r="B12" t="s">
         <v>1</v>
       </c>
@@ -4156,7 +4174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
       <c r="B13" t="s">
         <v>1</v>
       </c>
@@ -4188,7 +4206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.4">
       <c r="B14" t="s">
         <v>1</v>
       </c>
@@ -4220,7 +4238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.4">
       <c r="B15" t="s">
         <v>1</v>
       </c>
@@ -4240,7 +4258,7 @@
         <v>0</v>
       </c>
       <c r="H15" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15" t="s">
         <v>0</v>
@@ -4252,7 +4270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.4">
       <c r="B16" t="s">
         <v>1</v>
       </c>
@@ -4289,7 +4307,7 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" t="s">
         <v>0</v>
@@ -4414,7 +4432,7 @@
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B21" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" t="s">
         <v>0</v>
@@ -4761,7 +4779,7 @@
         <v>0</v>
       </c>
       <c r="K31" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.4">
@@ -7137,7 +7155,7 @@
         <v>0</v>
       </c>
       <c r="C106" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D106" t="s">
         <v>0</v>
@@ -7248,7 +7266,7 @@
         <v>0</v>
       </c>
       <c r="H109" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I109" t="s">
         <v>0</v>
@@ -7294,7 +7312,7 @@
     </row>
     <row r="111" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B111" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C111" t="s">
         <v>2</v>
@@ -7328,6 +7346,9 @@
       <c r="B112" t="s">
         <v>2</v>
       </c>
+      <c r="C112" t="s">
+        <v>2</v>
+      </c>
       <c r="D112" t="s">
         <v>0</v>
       </c>
@@ -7483,7 +7504,7 @@
         <v>0</v>
       </c>
       <c r="G117" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H117" t="s">
         <v>2</v>
@@ -7538,7 +7559,7 @@
         <v>0</v>
       </c>
       <c r="F119" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G119" t="s">
         <v>2</v>
@@ -7557,6 +7578,9 @@
       </c>
     </row>
     <row r="120" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B120" t="s">
+        <v>2</v>
+      </c>
       <c r="D120" t="s">
         <v>0</v>
       </c>
@@ -7567,6 +7591,9 @@
         <v>2</v>
       </c>
       <c r="G120" t="s">
+        <v>2</v>
+      </c>
+      <c r="H120" t="s">
         <v>2</v>
       </c>
       <c r="I120" t="s">
@@ -7632,6 +7659,9 @@
       <c r="E123" t="s">
         <v>0</v>
       </c>
+      <c r="F123" t="s">
+        <v>2</v>
+      </c>
       <c r="G123" t="s">
         <v>2</v>
       </c>
@@ -7707,7 +7737,7 @@
     </row>
     <row r="127" spans="2:11" x14ac:dyDescent="0.4">
       <c r="D127" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E127" t="s">
         <v>0</v>
@@ -7752,6 +7782,9 @@
       <c r="E129" t="s">
         <v>0</v>
       </c>
+      <c r="G129" t="s">
+        <v>2</v>
+      </c>
       <c r="I129" t="s">
         <v>0</v>
       </c>
@@ -7804,7 +7837,7 @@
         <v>0</v>
       </c>
       <c r="I132" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J132" t="s">
         <v>0</v>
@@ -7882,6 +7915,9 @@
       </c>
     </row>
     <row r="137" spans="4:11" x14ac:dyDescent="0.4">
+      <c r="D137" t="s">
+        <v>2</v>
+      </c>
       <c r="E137" t="s">
         <v>0</v>
       </c>
@@ -7983,6 +8019,9 @@
       <c r="E144" t="s">
         <v>0</v>
       </c>
+      <c r="I144" t="s">
+        <v>2</v>
+      </c>
       <c r="J144" t="s">
         <v>0</v>
       </c>
@@ -8014,7 +8053,7 @@
     </row>
     <row r="147" spans="5:11" x14ac:dyDescent="0.4">
       <c r="E147" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J147" t="s">
         <v>0</v>
@@ -8090,6 +8129,9 @@
       </c>
     </row>
     <row r="154" spans="5:11" x14ac:dyDescent="0.4">
+      <c r="E154" t="s">
+        <v>2</v>
+      </c>
       <c r="J154" t="s">
         <v>0</v>
       </c>
@@ -8387,7 +8429,7 @@
     </row>
     <row r="191" spans="10:11" x14ac:dyDescent="0.4">
       <c r="J191" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K191" t="s">
         <v>0</v>
@@ -8458,6 +8500,9 @@
       </c>
     </row>
     <row r="200" spans="10:11" x14ac:dyDescent="0.4">
+      <c r="J200" t="s">
+        <v>2</v>
+      </c>
       <c r="K200" t="s">
         <v>0</v>
       </c>
@@ -8474,7 +8519,7 @@
     </row>
     <row r="203" spans="10:11" x14ac:dyDescent="0.4">
       <c r="K203" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="204" spans="10:11" x14ac:dyDescent="0.4">
@@ -8572,10 +8617,15 @@
         <v>2</v>
       </c>
     </row>
+    <row r="223" spans="11:11" x14ac:dyDescent="0.4">
+      <c r="K223" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="B4:I161" xr:uid="{D83EDAD7-ABE3-4CBE-B6E6-396DDE8E1A3C}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="J3:J200">
-    <sortCondition ref="J3:J200"/>
+  <autoFilter ref="B5:I162" xr:uid="{D83EDAD7-ABE3-4CBE-B6E6-396DDE8E1A3C}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="J3:J201">
+    <sortCondition ref="J3:J201"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>